<commit_message>
add timer1 namespace and functions
</commit_message>
<xml_diff>
--- a/Doc/freq.xlsx
+++ b/Doc/freq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Montre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Montre\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>Mhz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Clock</t>
   </si>
@@ -48,6 +45,21 @@
   </si>
   <si>
     <t>iterations</t>
+  </si>
+  <si>
+    <t>TWBR</t>
+  </si>
+  <si>
+    <t>TWPS</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>F_CLK</t>
+  </si>
+  <si>
+    <t>MHz</t>
   </si>
 </sst>
 </file>
@@ -55,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,11 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,20 +427,20 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -435,28 +448,28 @@
         <v>1024</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <f>A1*1000/A2</f>
-        <v>7.8125</v>
+        <v>3.90625</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <f>1/(A3*1000)</f>
-        <v>1.2799999999999999E-4</v>
+        <v>2.5599999999999999E-4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -464,13 +477,13 @@
         <v>750</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
         <v>5000</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -479,14 +492,53 @@
         <v>5859.375</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <f>C7*A4</f>
-        <v>0.64</v>
+        <v>1.28</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <f>(B11*2/(B14/1000)-16)/2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
@@ -494,5 +546,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add timer0 namespace and functions
</commit_message>
<xml_diff>
--- a/Doc/freq.xlsx
+++ b/Doc/freq.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Clock</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Prescaler</t>
   </si>
   <si>
-    <t>sec</t>
-  </si>
-  <si>
     <t>ms</t>
   </si>
   <si>
@@ -60,15 +57,18 @@
   </si>
   <si>
     <t>MHz</t>
+  </si>
+  <si>
+    <t>interrupt</t>
+  </si>
+  <si>
+    <t>TWI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,12 +104,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,24 +428,27 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="5" width="10.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="3">
+      <c r="A1" s="2">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1024</v>
       </c>
       <c r="C2" t="s">
@@ -452,7 +456,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <f>A1*1000/A2</f>
         <v>3.90625</v>
       </c>
@@ -465,57 +469,68 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
-        <f>1/(A3*1000)</f>
-        <v>2.5599999999999999E-4</v>
+        <f>1/(A3)</f>
+        <v>0.25600000000000001</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>750</v>
       </c>
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>256</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
-        <f>A7*8000000/1024/1000</f>
-        <v>5859.375</v>
+        <f>A7*A1*1000000/A2/1000</f>
+        <v>2929.6875</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <f>C7*A4</f>
-        <v>1.28</v>
+        <v>65.536000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <f>A1</f>
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <f>(B11*2/(B14/1000)-16)/2</f>
@@ -524,7 +539,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -532,9 +547,9 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="4">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5">
         <v>100</v>
       </c>
       <c r="C14" t="s">
@@ -542,7 +557,7 @@
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="2"/>
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add timer namespaces and functions -- make them classes?
</commit_message>
<xml_diff>
--- a/Doc/freq.xlsx
+++ b/Doc/freq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Montre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Montre\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>Mhz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Clock</t>
   </si>
@@ -41,22 +38,37 @@
     <t>Prescaler</t>
   </si>
   <si>
-    <t>sec</t>
-  </si>
-  <si>
     <t>ms</t>
   </si>
   <si>
     <t>iterations</t>
+  </si>
+  <si>
+    <t>TWBR</t>
+  </si>
+  <si>
+    <t>TWPS</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>F_CLK</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>interrupt</t>
+  </si>
+  <si>
+    <t>TWI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,11 +104,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,85 +428,139 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="5" width="10.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="3">
-        <v>8</v>
+      <c r="A1" s="2">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
+        <f>A1*1000/A2</f>
+        <v>3.90625</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
-        <v>1024</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <f>A1*1000/A2</f>
-        <v>7.8125</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
-        <f>1/(A3*1000)</f>
-        <v>1.2799999999999999E-4</v>
+        <f>1/(A3)</f>
+        <v>0.25600000000000001</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>750</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>256</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
-        <v>750</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
-        <f>A7*8000000/1024/1000</f>
-        <v>5859.375</v>
+        <f>A7*A1*1000000/A2/1000</f>
+        <v>2929.6875</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <f>C7*A4</f>
-        <v>0.64</v>
+        <v>65.536000000000001</v>
       </c>
       <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <f>A1</f>
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
+      <c r="B12">
+        <f>(B11*2/(B14/1000)-16)/2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="2"/>
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
move src files to src directory
</commit_message>
<xml_diff>
--- a/Doc/freq.xlsx
+++ b/Doc/freq.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Clock</t>
   </si>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -436,7 +436,7 @@
     <col min="1" max="5" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2">
         <v>4</v>
       </c>
@@ -447,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1024</v>
       </c>
@@ -455,7 +455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <f>A1*1000/A2</f>
         <v>3.90625</v>
@@ -467,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <f>1/(A3)</f>
         <v>0.25600000000000001</v>
@@ -476,12 +476,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>750</v>
       </c>
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <f>A7*A1*1000000/A2/1000</f>
         <v>2929.6875</v>
@@ -511,41 +511,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <f>A1</f>
-        <v>4</v>
+        <f>A1*2</f>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12">
-        <f>(B11*2/(B14/1000)-16)/2</f>
+        <f>(B11/(B14/1000)-16)/2</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D12" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D13">
+        <f>B13</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -553,6 +566,13 @@
         <v>100</v>
       </c>
       <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f>D11*1000/(16+(2*D13*D12))</f>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="E14" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
main now contains a test for the 12:00 led
</commit_message>
<xml_diff>
--- a/Doc/freq.xlsx
+++ b/Doc/freq.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Montre\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\watch\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13238" windowHeight="6570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13238" windowHeight="6570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Clock</t>
   </si>
@@ -63,12 +64,24 @@
   </si>
   <si>
     <t>TWI</t>
+  </si>
+  <si>
+    <t>F_CPU</t>
+  </si>
+  <si>
+    <t>F_TWI</t>
+  </si>
+  <si>
+    <t>Counter/timer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,13 +117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -583,4 +597,196 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="5" width="10.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
+        <f>A2*1000/A3</f>
+        <v>0.9765625</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <f>1/(A4)</f>
+        <v>1.024</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <v>750</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>256</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <f>A8*A2*1000000/A3/1000</f>
+        <v>732.421875</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>C8*A5</f>
+        <v>262.14400000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G10">
+        <f>MAX((G7/G8-16)/2,10)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4">
+        <f>A2*B11</f>
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <f>(B12/(B15/1000)-16)/2</f>
+        <v>1.0909090909090917</v>
+      </c>
+      <c r="D13" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>B14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <f>D12*1000/(16+(2*D14*D13))</f>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f>1000000/(16+(2*10*1))</f>
+        <v>27777.777777777777</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>